<commit_message>
Fix lỗi check và tăng thời gian timeout
</commit_message>
<xml_diff>
--- a/temp/Getsu/Resources/ExportExcel.xlsx
+++ b/temp/Getsu/Resources/ExportExcel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>3.年</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Tên file ảnh (Đường dẫn\tên batch\tên file ảnh)</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -421,13 +424,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF1"/>
+  <dimension ref="A1:BG1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="BG1" sqref="BG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +440,7 @@
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -609,6 +612,9 @@
       </c>
       <c r="BF1" s="5">
         <v>25</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>